<commit_message>
finish check over crop.py and sorting inputs. Plus sire mating function and mortality for sheep.py
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -430,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -553,7 +553,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -562,38 +562,15 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -604,7 +581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -700,45 +677,23 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
check crop inputs and add a couple more rotations.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="40">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -36,6 +36,39 @@
     <t>YYENEr</t>
   </si>
   <si>
+    <t>YYNEEr</t>
+  </si>
+  <si>
+    <t>YYEENw</t>
+  </si>
+  <si>
+    <t>YYENEb</t>
+  </si>
+  <si>
+    <t>AAAAAz</t>
+  </si>
+  <si>
+    <t>AAAANw</t>
+  </si>
+  <si>
+    <t>AAANEb</t>
+  </si>
+  <si>
+    <t>AANEEa</t>
+  </si>
+  <si>
+    <t>AYEEAa</t>
+  </si>
+  <si>
+    <t>YYEAAa</t>
+  </si>
+  <si>
+    <t>YYAAAa</t>
+  </si>
+  <si>
+    <t>YAAAAa</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -60,6 +93,9 @@
     <t>r</t>
   </si>
   <si>
+    <t>w</t>
+  </si>
+  <si>
     <t>AYAEA</t>
   </si>
   <si>
@@ -72,7 +108,34 @@
     <t>YYNEN</t>
   </si>
   <si>
+    <t>YYEEN</t>
+  </si>
+  <si>
+    <t>YYNEE</t>
+  </si>
+  <si>
     <t>AAAAA</t>
+  </si>
+  <si>
+    <t>AAAAN</t>
+  </si>
+  <si>
+    <t>AAANE</t>
+  </si>
+  <si>
+    <t>AANEE</t>
+  </si>
+  <si>
+    <t>AYEEA</t>
+  </si>
+  <si>
+    <t>YYEAA</t>
+  </si>
+  <si>
+    <t>YYAAA</t>
+  </si>
+  <si>
+    <t>YAAAA</t>
   </si>
 </sst>
 </file>
@@ -430,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,22 +504,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -464,22 +527,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -487,22 +550,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -510,22 +573,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -533,22 +596,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -556,22 +619,275 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +897,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -592,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -603,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -614,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -625,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -636,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -647,7 +963,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -658,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -669,7 +985,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -680,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -691,10 +1007,252 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +1262,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -712,102 +1270,282 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add inputs for fodder. rerun stubble sim.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,33 +17,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="71">
   <si>
     <t>AAAAAa</t>
   </si>
   <si>
-    <t>YAEAEa</t>
+    <t>YAEAE1a</t>
   </si>
   <si>
     <t>AYAEAb</t>
   </si>
   <si>
+    <t>YAEAOFa</t>
+  </si>
+  <si>
+    <t>AYAEAof</t>
+  </si>
+  <si>
     <t>YYNENb</t>
   </si>
   <si>
-    <t>YYENEz</t>
-  </si>
-  <si>
-    <t>YYENEr</t>
-  </si>
-  <si>
-    <t>YYNEEr</t>
+    <t>YYENE1z</t>
+  </si>
+  <si>
+    <t>YYENE1r</t>
+  </si>
+  <si>
+    <t>YYNEE1r</t>
   </si>
   <si>
     <t>YYEENw</t>
   </si>
   <si>
-    <t>YYENEb</t>
+    <t>YYENE1b</t>
   </si>
   <si>
     <t>AAAAAz</t>
@@ -52,10 +58,10 @@
     <t>AAAANw</t>
   </si>
   <si>
-    <t>AAANEb</t>
-  </si>
-  <si>
-    <t>AANEEa</t>
+    <t>AAANE1b</t>
+  </si>
+  <si>
+    <t>AANEE1a</t>
   </si>
   <si>
     <t>AYEEAa</t>
@@ -70,13 +76,13 @@
     <t>YAAAAa</t>
   </si>
   <si>
-    <t>YYENEl</t>
+    <t>YYENE1l</t>
   </si>
   <si>
     <t>YYPENw</t>
   </si>
   <si>
-    <t>YYEPEz</t>
+    <t>YYEPE1z</t>
   </si>
   <si>
     <t>YYNEPw</t>
@@ -91,7 +97,7 @@
     <t>AAAEAa</t>
   </si>
   <si>
-    <t>YAAAEa</t>
+    <t>YAAAE1a</t>
   </si>
   <si>
     <t>YAAANw</t>
@@ -106,7 +112,7 @@
     <t>AANEAa</t>
   </si>
   <si>
-    <t>AAANEa</t>
+    <t>AAANE1a</t>
   </si>
   <si>
     <t>A</t>
@@ -124,12 +130,21 @@
     <t>P</t>
   </si>
   <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
   </si>
   <si>
+    <t>of</t>
+  </si>
+  <si>
     <t>z</t>
   </si>
   <si>
@@ -145,19 +160,22 @@
     <t>AAAAA</t>
   </si>
   <si>
-    <t>YAEAE</t>
+    <t>YAEAE1</t>
   </si>
   <si>
     <t>AYAEA</t>
   </si>
   <si>
+    <t>YAEAOF</t>
+  </si>
+  <si>
     <t>YYNEN</t>
   </si>
   <si>
-    <t>YYENE</t>
-  </si>
-  <si>
-    <t>YYNEE</t>
+    <t>YYENE1</t>
+  </si>
+  <si>
+    <t>YYNEE1</t>
   </si>
   <si>
     <t>YYEEN</t>
@@ -166,10 +184,10 @@
     <t>AAAAN</t>
   </si>
   <si>
-    <t>AAANE</t>
-  </si>
-  <si>
-    <t>AANEE</t>
+    <t>AAANE1</t>
+  </si>
+  <si>
+    <t>AANEE1</t>
   </si>
   <si>
     <t>AYEEA</t>
@@ -187,7 +205,7 @@
     <t>YYPEN</t>
   </si>
   <si>
-    <t>YYEPE</t>
+    <t>YYEPE1</t>
   </si>
   <si>
     <t>YYNEP</t>
@@ -202,7 +220,7 @@
     <t>AAAEA</t>
   </si>
   <si>
-    <t>YAAAE</t>
+    <t>YAAAE1</t>
   </si>
   <si>
     <t>YAAAN</t>
@@ -569,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,22 +598,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -603,22 +621,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -626,22 +644,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -649,22 +667,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -672,22 +690,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -695,22 +713,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -718,22 +736,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -741,22 +759,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -764,22 +782,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -787,22 +805,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -810,22 +828,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -833,22 +851,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -856,22 +874,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -879,22 +897,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -902,22 +920,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -925,22 +943,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -948,22 +966,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -971,22 +989,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -994,19 +1012,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" t="s">
         <v>39</v>
@@ -1017,22 +1035,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1040,22 +1058,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1063,22 +1081,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1086,22 +1104,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1109,22 +1127,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1132,22 +1150,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
         <v>32</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1155,19 +1173,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
         <v>39</v>
@@ -1178,22 +1196,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1201,22 +1219,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1224,22 +1242,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
         <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1247,22 +1265,68 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
-        <v>35</v>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1336,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1283,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1294,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1305,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1316,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1327,7 +1391,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1338,7 +1402,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1349,7 +1413,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1360,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1371,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1382,7 +1446,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1393,7 +1457,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1404,7 +1468,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1415,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1426,7 +1490,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1437,7 +1501,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1448,7 +1512,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1459,7 +1523,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1470,7 +1534,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1481,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1492,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1503,7 +1567,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1514,7 +1578,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1525,7 +1589,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1536,7 +1600,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1547,7 +1611,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1558,7 +1622,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1569,7 +1633,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1580,7 +1644,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1602,9 +1666,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
     </row>
@@ -1615,7 +1701,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1626,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1637,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1648,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1659,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1670,7 +1756,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1681,7 +1767,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -1692,7 +1778,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -1703,7 +1789,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1714,7 +1800,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1725,7 +1811,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1736,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1747,7 +1833,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1758,7 +1844,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1769,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1780,7 +1866,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1791,7 +1877,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1802,7 +1888,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1813,7 +1899,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1824,7 +1910,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1835,7 +1921,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1846,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1868,7 +1954,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1879,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1890,7 +1976,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1901,7 +1987,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1912,7 +1998,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -1923,7 +2009,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -1934,7 +2020,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -1945,9 +2031,31 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
         <v>-1</v>
       </c>
     </row>
@@ -1958,7 +2066,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1966,482 +2074,502 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dry sowing rotation.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="73">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -28,6 +28,9 @@
     <t>AYAEAb</t>
   </si>
   <si>
+    <t>AYAEAbd</t>
+  </si>
+  <si>
     <t>YAEAOFa</t>
   </si>
   <si>
@@ -140,6 +143,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>bd</t>
   </si>
   <si>
     <t>of</t>
@@ -587,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,22 +604,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -621,22 +627,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -644,22 +650,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -670,19 +676,19 @@
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -690,22 +696,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -716,19 +722,19 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -736,22 +742,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -759,22 +765,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -782,22 +788,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -805,22 +811,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -828,22 +834,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -851,22 +857,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -874,19 +880,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
         <v>44</v>
@@ -897,22 +903,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -920,22 +926,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -943,22 +949,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -969,19 +975,19 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -989,22 +995,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1012,22 +1018,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1035,22 +1041,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1058,22 +1064,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1081,22 +1087,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1104,19 +1110,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
         <v>44</v>
@@ -1127,22 +1133,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1150,22 +1156,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1173,22 +1179,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1199,19 +1205,19 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1219,22 +1225,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1242,22 +1248,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1265,22 +1271,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1288,22 +1294,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1311,22 +1317,45 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" t="s">
-        <v>39</v>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1365,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1347,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1358,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1369,7 +1398,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1380,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1391,7 +1420,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1413,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1424,7 +1453,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1435,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1446,7 +1475,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1457,7 +1486,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1468,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1479,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1490,7 +1519,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1501,7 +1530,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1512,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1523,7 +1552,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1534,7 +1563,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1545,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1556,7 +1585,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1567,7 +1596,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1578,7 +1607,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1589,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1600,7 +1629,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1611,7 +1640,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1622,7 +1651,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1633,7 +1662,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1644,7 +1673,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1655,7 +1684,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1666,7 +1695,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1677,7 +1706,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1688,9 +1717,20 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33">
         <v>1</v>
       </c>
     </row>
@@ -1701,7 +1741,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1712,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1723,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1734,7 +1774,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1745,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1756,7 +1796,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1778,7 +1818,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -1789,7 +1829,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1800,7 +1840,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1811,7 +1851,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1822,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1844,7 +1884,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1855,7 +1895,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1866,7 +1906,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1877,7 +1917,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1888,7 +1928,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1899,7 +1939,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1910,7 +1950,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1921,7 +1961,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1932,7 +1972,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1943,7 +1983,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1954,7 +1994,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1965,7 +2005,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1976,7 +2016,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1987,7 +2027,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1998,7 +2038,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2009,7 +2049,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2020,7 +2060,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2031,7 +2071,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2042,7 +2082,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2053,9 +2093,20 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33">
         <v>-1</v>
       </c>
     </row>
@@ -2074,502 +2125,502 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alter rotationgeneration after talking to Tim: less crop clustering because need to track yrs since same crop for disease.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,42 +17,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="77">
   <si>
     <t>AAAAAa</t>
   </si>
   <si>
-    <t>YAEAE1a</t>
-  </si>
-  <si>
-    <t>AYAEAb</t>
-  </si>
-  <si>
-    <t>AYAEAbd</t>
-  </si>
-  <si>
-    <t>YAEAOFa</t>
-  </si>
-  <si>
-    <t>AYAEAof</t>
-  </si>
-  <si>
-    <t>YYNENb</t>
-  </si>
-  <si>
-    <t>YYENE1z</t>
-  </si>
-  <si>
-    <t>YYENE1r</t>
-  </si>
-  <si>
-    <t>YYNEE1r</t>
-  </si>
-  <si>
-    <t>YYEENw</t>
-  </si>
-  <si>
-    <t>YYENE1b</t>
+    <t>YABABa</t>
+  </si>
+  <si>
+    <t>AYABAb</t>
+  </si>
+  <si>
+    <t>AYABAbd</t>
+  </si>
+  <si>
+    <t>YAOAOFa</t>
+  </si>
+  <si>
+    <t>AYAOAof</t>
+  </si>
+  <si>
+    <t>YYNBNb</t>
+  </si>
+  <si>
+    <t>YYBNBz</t>
+  </si>
+  <si>
+    <t>YYBNBr</t>
+  </si>
+  <si>
+    <t>YYNWBr</t>
+  </si>
+  <si>
+    <t>YYWBNw</t>
+  </si>
+  <si>
+    <t>YYBNWb</t>
   </si>
   <si>
     <t>AAAAAz</t>
@@ -61,16 +61,16 @@
     <t>AAAANw</t>
   </si>
   <si>
-    <t>AAANE1b</t>
-  </si>
-  <si>
-    <t>AANEE1a</t>
-  </si>
-  <si>
-    <t>AYEEAa</t>
-  </si>
-  <si>
-    <t>YYEAAa</t>
+    <t>AAANWb</t>
+  </si>
+  <si>
+    <t>AANWBa</t>
+  </si>
+  <si>
+    <t>AYWBAa</t>
+  </si>
+  <si>
+    <t>YYBAAa</t>
   </si>
   <si>
     <t>YYAAAa</t>
@@ -79,28 +79,28 @@
     <t>YAAAAa</t>
   </si>
   <si>
-    <t>YYENE1l</t>
-  </si>
-  <si>
-    <t>YYPENw</t>
-  </si>
-  <si>
-    <t>YYEPE1z</t>
-  </si>
-  <si>
-    <t>YYNEPw</t>
+    <t>YYWNWl</t>
+  </si>
+  <si>
+    <t>YYLWNw</t>
+  </si>
+  <si>
+    <t>YYWLWz</t>
+  </si>
+  <si>
+    <t>YYNWLw</t>
   </si>
   <si>
     <t>AYAAAw</t>
   </si>
   <si>
-    <t>AAEAAa</t>
-  </si>
-  <si>
-    <t>AAAEAa</t>
-  </si>
-  <si>
-    <t>YAAAE1a</t>
+    <t>AAWAAa</t>
+  </si>
+  <si>
+    <t>AAAWAa</t>
+  </si>
+  <si>
+    <t>YAAAWa</t>
   </si>
   <si>
     <t>YAAANw</t>
@@ -109,13 +109,13 @@
     <t>AYAAAz</t>
   </si>
   <si>
-    <t>AYEAAa</t>
-  </si>
-  <si>
-    <t>AANEAa</t>
-  </si>
-  <si>
-    <t>AAANE1a</t>
+    <t>AYWAAa</t>
+  </si>
+  <si>
+    <t>AANWAa</t>
+  </si>
+  <si>
+    <t>AAANWa</t>
   </si>
   <si>
     <t>A</t>
@@ -124,16 +124,19 @@
     <t>Y</t>
   </si>
   <si>
-    <t>E</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>E1</t>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>OF</t>
@@ -166,40 +169,46 @@
     <t>AAAAA</t>
   </si>
   <si>
-    <t>YAEAE1</t>
-  </si>
-  <si>
-    <t>AYAEA</t>
-  </si>
-  <si>
-    <t>YAEAOF</t>
-  </si>
-  <si>
-    <t>YYNEN</t>
-  </si>
-  <si>
-    <t>YYENE1</t>
-  </si>
-  <si>
-    <t>YYNEE1</t>
-  </si>
-  <si>
-    <t>YYEEN</t>
+    <t>YABAB</t>
+  </si>
+  <si>
+    <t>AYABA</t>
+  </si>
+  <si>
+    <t>YAOAOF</t>
+  </si>
+  <si>
+    <t>AYAOA</t>
+  </si>
+  <si>
+    <t>YYNBN</t>
+  </si>
+  <si>
+    <t>YYBNB</t>
+  </si>
+  <si>
+    <t>YYNWB</t>
+  </si>
+  <si>
+    <t>YYWBN</t>
+  </si>
+  <si>
+    <t>YYBNW</t>
   </si>
   <si>
     <t>AAAAN</t>
   </si>
   <si>
-    <t>AAANE1</t>
-  </si>
-  <si>
-    <t>AANEE1</t>
-  </si>
-  <si>
-    <t>AYEEA</t>
-  </si>
-  <si>
-    <t>YYEAA</t>
+    <t>AAANW</t>
+  </si>
+  <si>
+    <t>AANWB</t>
+  </si>
+  <si>
+    <t>AYWBA</t>
+  </si>
+  <si>
+    <t>YYBAA</t>
   </si>
   <si>
     <t>YYAAA</t>
@@ -208,34 +217,37 @@
     <t>YAAAA</t>
   </si>
   <si>
-    <t>YYPEN</t>
-  </si>
-  <si>
-    <t>YYEPE1</t>
-  </si>
-  <si>
-    <t>YYNEP</t>
+    <t>YYWNW</t>
+  </si>
+  <si>
+    <t>YYLWN</t>
+  </si>
+  <si>
+    <t>YYWLW</t>
+  </si>
+  <si>
+    <t>YYNWL</t>
   </si>
   <si>
     <t>AYAAA</t>
   </si>
   <si>
-    <t>AAEAA</t>
-  </si>
-  <si>
-    <t>AAAEA</t>
-  </si>
-  <si>
-    <t>YAAAE1</t>
+    <t>AAWAA</t>
+  </si>
+  <si>
+    <t>AAAWA</t>
+  </si>
+  <si>
+    <t>YAAAW</t>
   </si>
   <si>
     <t>YAAAN</t>
   </si>
   <si>
-    <t>AYEAA</t>
-  </si>
-  <si>
-    <t>AANEA</t>
+    <t>AYWAA</t>
+  </si>
+  <si>
+    <t>AANWA</t>
   </si>
 </sst>
 </file>
@@ -619,7 +631,7 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -639,10 +651,10 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -665,7 +677,7 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -688,7 +700,7 @@
         <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -702,16 +714,16 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -728,13 +740,13 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -748,16 +760,16 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -774,13 +786,13 @@
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -797,13 +809,13 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -817,16 +829,16 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -840,16 +852,16 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -866,13 +878,13 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -895,7 +907,7 @@
         <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -915,10 +927,10 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -935,13 +947,13 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -955,16 +967,16 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
-        <v>38</v>
-      </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -978,7 +990,7 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -987,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1010,7 +1022,7 @@
         <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1033,7 +1045,7 @@
         <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1056,7 +1068,7 @@
         <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1070,16 +1082,16 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F21" t="s">
         <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1093,16 +1105,16 @@
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1116,16 +1128,16 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
         <v>38</v>
       </c>
       <c r="G23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1139,16 +1151,16 @@
         <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1171,7 +1183,7 @@
         <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1185,7 +1197,7 @@
         <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -1194,7 +1206,7 @@
         <v>33</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1211,13 +1223,13 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
         <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1240,7 +1252,7 @@
         <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1260,10 +1272,10 @@
         <v>33</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1286,7 +1298,7 @@
         <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1300,7 +1312,7 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E31" t="s">
         <v>33</v>
@@ -1309,7 +1321,7 @@
         <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1323,16 +1335,16 @@
         <v>33</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F32" t="s">
         <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1349,13 +1361,13 @@
         <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F33" t="s">
         <v>38</v>
       </c>
       <c r="G33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1387,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1398,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1409,7 +1421,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1420,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1431,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1442,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1453,7 +1465,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1464,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1475,7 +1487,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1486,7 +1498,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1497,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1508,7 +1520,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1519,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1530,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1541,7 +1553,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1552,7 +1564,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1563,7 +1575,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1574,7 +1586,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1585,7 +1597,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1596,7 +1608,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1607,7 +1619,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1618,7 +1630,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1629,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1640,7 +1652,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1651,7 +1663,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1662,7 +1674,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1673,7 +1685,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1684,7 +1696,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1695,7 +1707,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1706,7 +1718,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1717,7 +1729,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1728,7 +1740,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1752,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1763,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1774,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1785,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1796,7 +1808,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1807,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -1818,7 +1830,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -1829,7 +1841,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1840,7 +1852,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1851,7 +1863,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1862,7 +1874,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1873,7 +1885,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1884,7 +1896,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1895,7 +1907,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1906,7 +1918,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1917,7 +1929,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1928,7 +1940,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1939,7 +1951,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1950,7 +1962,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1961,7 +1973,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1972,7 +1984,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1983,7 +1995,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1994,7 +2006,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2005,7 +2017,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2016,7 +2028,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2027,7 +2039,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2038,7 +2050,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2049,7 +2061,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2060,7 +2072,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2071,7 +2083,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2082,7 +2094,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2093,7 +2105,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2104,7 +2116,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2117,7 +2129,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2125,7 +2137,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -2145,7 +2157,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -2160,12 +2172,12 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -2177,15 +2189,15 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -2197,15 +2209,15 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -2214,10 +2226,10 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
@@ -2225,7 +2237,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -2234,18 +2246,18 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -2254,18 +2266,18 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -2285,7 +2297,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2305,7 +2317,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -2314,10 +2326,10 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -2325,7 +2337,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -2334,10 +2346,10 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
@@ -2348,16 +2360,16 @@
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>33</v>
@@ -2365,7 +2377,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -2380,12 +2392,12 @@
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -2400,12 +2412,12 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -2414,7 +2426,7 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -2425,7 +2437,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -2440,32 +2452,32 @@
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -2474,7 +2486,7 @@
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
@@ -2485,7 +2497,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -2497,15 +2509,15 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
@@ -2517,15 +2529,15 @@
         <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -2545,7 +2557,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
@@ -2554,18 +2566,18 @@
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -2574,18 +2586,18 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>34</v>
@@ -2594,18 +2606,18 @@
         <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
         <v>35</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -2617,10 +2629,70 @@
         <v>37</v>
       </c>
       <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
         <v>35</v>
       </c>
-      <c r="F25" t="s">
-        <v>36</v>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add faba rotation based on Tims 2019 info. No profit change
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="86">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -79,6 +79,18 @@
     <t>YAAAAa</t>
   </si>
   <si>
+    <t>YYFWBz</t>
+  </si>
+  <si>
+    <t>YYBNWf</t>
+  </si>
+  <si>
+    <t>YYNWFw</t>
+  </si>
+  <si>
+    <t>YYWFWb</t>
+  </si>
+  <si>
     <t>YYWNWl</t>
   </si>
   <si>
@@ -136,6 +148,9 @@
     <t>W</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>L</t>
   </si>
   <si>
@@ -163,6 +178,9 @@
     <t>w</t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>l</t>
   </si>
   <si>
@@ -215,6 +233,15 @@
   </si>
   <si>
     <t>YAAAA</t>
+  </si>
+  <si>
+    <t>YYFWB</t>
+  </si>
+  <si>
+    <t>YYNWF</t>
+  </si>
+  <si>
+    <t>YYWFW</t>
   </si>
   <si>
     <t>YYWNW</t>
@@ -605,7 +632,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -616,22 +643,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -639,22 +666,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -662,22 +689,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -685,22 +712,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -708,22 +735,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -731,22 +758,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -754,22 +781,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -777,22 +804,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -800,22 +827,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -823,22 +850,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -846,22 +873,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -869,22 +896,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -892,22 +919,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -915,22 +942,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -938,22 +965,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -961,22 +988,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -984,22 +1011,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1007,22 +1034,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1030,22 +1057,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1053,22 +1080,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1076,22 +1103,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1099,22 +1126,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1122,22 +1149,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1145,19 +1172,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
         <v>47</v>
@@ -1168,22 +1195,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1191,22 +1218,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1214,22 +1241,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1237,22 +1264,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1260,22 +1287,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F29" t="s">
         <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1283,22 +1310,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1306,22 +1333,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1329,22 +1356,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1352,22 +1379,114 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" t="s">
-        <v>41</v>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1496,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1388,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1399,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1410,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1421,7 +1540,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1432,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1443,7 +1562,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1454,7 +1573,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1465,7 +1584,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1476,7 +1595,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1487,7 +1606,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1498,7 +1617,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1509,7 +1628,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1520,7 +1639,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1531,7 +1650,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1542,7 +1661,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1553,7 +1672,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1564,7 +1683,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1575,7 +1694,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1586,7 +1705,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1597,7 +1716,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1608,7 +1727,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1619,7 +1738,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1630,7 +1749,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1641,7 +1760,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1652,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1663,7 +1782,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1674,7 +1793,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1685,7 +1804,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1696,7 +1815,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1707,7 +1826,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1718,7 +1837,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1729,7 +1848,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1740,9 +1859,53 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37">
         <v>1</v>
       </c>
     </row>
@@ -1753,7 +1916,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1764,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1775,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1786,7 +1949,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1797,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1808,7 +1971,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1819,7 +1982,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -1830,7 +1993,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -1841,7 +2004,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1852,7 +2015,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1863,7 +2026,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1874,7 +2037,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1885,7 +2048,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1896,7 +2059,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1907,7 +2070,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1918,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1929,7 +2092,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1940,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1951,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1962,7 +2125,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1973,7 +2136,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1984,7 +2147,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1995,7 +2158,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2006,7 +2169,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2017,7 +2180,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2028,7 +2191,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2039,7 +2202,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2050,7 +2213,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2061,7 +2224,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2072,7 +2235,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2083,7 +2246,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2094,7 +2257,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2105,7 +2268,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2116,9 +2279,53 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37">
         <v>-1</v>
       </c>
     </row>
@@ -2129,7 +2336,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2137,499 +2344,499 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
         <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
         <v>39</v>
@@ -2637,62 +2844,122 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the saltland pasture phase (SP)
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,11 +17,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
   <si>
     <t>AAAAAa</t>
   </si>
   <si>
+    <t>SPSPSPSPSPsp</t>
+  </si>
+  <si>
     <t>YABABa</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t>A</t>
   </si>
   <si>
+    <t>SP</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -160,6 +166,9 @@
     <t>a</t>
   </si>
   <si>
+    <t>sp</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
@@ -185,6 +194,9 @@
   </si>
   <si>
     <t>AAAAA</t>
+  </si>
+  <si>
+    <t>SPSPSPSPSP</t>
   </si>
   <si>
     <t>YABAB</t>
@@ -632,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -643,22 +655,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -666,22 +678,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -689,22 +701,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -712,22 +724,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -738,19 +750,19 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -758,22 +770,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -784,19 +796,19 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -804,19 +816,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
@@ -827,22 +839,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -850,22 +862,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -873,22 +885,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -896,22 +908,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -919,19 +931,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
         <v>50</v>
@@ -942,22 +954,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -965,22 +977,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -988,22 +1000,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1011,22 +1023,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1037,19 +1049,19 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1057,22 +1069,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1080,22 +1092,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1103,22 +1115,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1126,19 +1138,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
         <v>41</v>
-      </c>
-      <c r="F22" t="s">
-        <v>42</v>
       </c>
       <c r="G22" t="s">
         <v>53</v>
@@ -1149,22 +1161,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1172,22 +1184,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1195,22 +1207,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1218,22 +1230,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1241,22 +1253,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1264,22 +1276,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1287,22 +1299,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1310,22 +1322,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1333,22 +1345,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1359,19 +1371,19 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1379,22 +1391,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1402,22 +1414,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1425,22 +1437,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G35" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1448,22 +1460,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G36" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1471,22 +1483,45 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" t="s">
-        <v>46</v>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1507,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1518,7 +1553,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1529,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1540,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1551,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1562,7 +1597,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1573,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1584,7 +1619,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1595,7 +1630,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1606,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1617,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1628,7 +1663,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1639,7 +1674,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1650,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1661,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1672,7 +1707,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1683,7 +1718,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1694,7 +1729,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1705,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1716,7 +1751,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1727,7 +1762,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1738,7 +1773,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1749,7 +1784,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1760,7 +1795,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1771,7 +1806,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1782,7 +1817,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1793,7 +1828,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1804,7 +1839,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1815,7 +1850,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1826,7 +1861,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1837,7 +1872,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1848,7 +1883,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1859,7 +1894,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1870,7 +1905,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1881,7 +1916,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1892,7 +1927,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1903,9 +1938,20 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
     </row>
@@ -1916,7 +1962,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1927,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1938,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1949,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1960,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1971,7 +2017,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1982,7 +2028,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -1993,7 +2039,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2004,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2015,7 +2061,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2026,7 +2072,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2037,7 +2083,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2048,7 +2094,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2059,7 +2105,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2070,7 +2116,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2081,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2092,7 +2138,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2103,7 +2149,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2114,7 +2160,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2125,7 +2171,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2136,7 +2182,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2147,7 +2193,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2158,7 +2204,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2169,7 +2215,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2180,7 +2226,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2191,7 +2237,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2202,7 +2248,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2213,7 +2259,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2224,7 +2270,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2235,7 +2281,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2246,7 +2292,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2257,7 +2303,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2268,7 +2314,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2279,7 +2325,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2290,7 +2336,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -2301,7 +2347,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -2312,7 +2358,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -2323,9 +2369,20 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38">
         <v>-1</v>
       </c>
     </row>
@@ -2336,7 +2393,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2344,442 +2401,442 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
         <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s">
         <v>41</v>
-      </c>
-      <c r="F21" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2787,16 +2844,16 @@
         <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
@@ -2804,162 +2861,182 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
         <v>41</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update rot.xl for cwm
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="81">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -82,18 +82,6 @@
     <t>YAAAAa</t>
   </si>
   <si>
-    <t>YYFWBz</t>
-  </si>
-  <si>
-    <t>YYBNWf</t>
-  </si>
-  <si>
-    <t>YYNWFw</t>
-  </si>
-  <si>
-    <t>YYWFWb</t>
-  </si>
-  <si>
     <t>YYWNWl</t>
   </si>
   <si>
@@ -154,9 +142,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -245,15 +227,6 @@
   </si>
   <si>
     <t>YAAAA</t>
-  </si>
-  <si>
-    <t>YYFWB</t>
-  </si>
-  <si>
-    <t>YYNWF</t>
-  </si>
-  <si>
-    <t>YYWFW</t>
   </si>
   <si>
     <t>YYWNW</t>
@@ -644,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,22 +628,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -678,22 +651,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -701,22 +674,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -724,22 +697,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -747,22 +720,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -770,22 +743,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -793,22 +766,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -816,22 +789,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -839,22 +812,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -862,22 +835,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -885,22 +858,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -908,22 +881,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -931,22 +904,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -954,22 +927,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -977,22 +950,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1000,22 +973,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1023,22 +996,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
         <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1046,22 +1019,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1069,22 +1042,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1092,22 +1065,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1115,22 +1088,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1138,22 +1111,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1161,22 +1134,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1184,22 +1157,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1207,19 +1180,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
         <v>50</v>
@@ -1230,22 +1203,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1253,22 +1226,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
         <v>43</v>
-      </c>
-      <c r="G27" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1276,22 +1249,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G28" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1299,22 +1272,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" t="s">
         <v>43</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1322,22 +1295,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1345,19 +1318,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G31" t="s">
         <v>48</v>
@@ -1368,22 +1341,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1391,22 +1364,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1414,114 +1387,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
         <v>43</v>
-      </c>
-      <c r="G34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" t="s">
-        <v>44</v>
-      </c>
-      <c r="G38" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1412,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1542,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1553,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1564,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1575,7 +1456,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1586,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1597,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1608,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1619,7 +1500,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1630,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1641,7 +1522,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1652,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1663,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1674,7 +1555,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1685,7 +1566,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1696,7 +1577,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1707,7 +1588,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1718,7 +1599,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1729,7 +1610,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1740,7 +1621,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1751,7 +1632,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1762,7 +1643,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1773,7 +1654,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1784,7 +1665,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1795,7 +1676,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1806,7 +1687,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1817,7 +1698,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1828,7 +1709,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1839,7 +1720,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1850,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1861,7 +1742,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1872,7 +1753,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1883,7 +1764,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1894,7 +1775,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1905,53 +1786,9 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38">
         <v>1</v>
       </c>
     </row>
@@ -1962,7 +1799,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1973,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1984,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1995,7 +1832,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2006,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2017,7 +1854,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2028,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2039,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2050,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2061,7 +1898,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2072,7 +1909,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2083,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2094,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2105,7 +1942,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2116,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2127,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2138,7 +1975,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2149,7 +1986,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2160,7 +1997,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2171,7 +2008,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2182,7 +2019,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2193,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2204,7 +2041,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2215,7 +2052,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2226,7 +2063,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2237,7 +2074,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2248,7 +2085,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2259,7 +2096,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2270,7 +2107,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2281,7 +2118,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2292,7 +2129,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2303,7 +2140,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2314,7 +2151,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2325,7 +2162,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2336,53 +2173,9 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38">
         <v>-1</v>
       </c>
     </row>
@@ -2393,7 +2186,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2401,519 +2194,519 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
         <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F26" t="s">
         <v>41</v>
@@ -2921,122 +2714,62 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make it so that the selection of which pinp to use is done via exp.xl
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="81">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -82,18 +82,6 @@
     <t>YAAAAa</t>
   </si>
   <si>
-    <t>YYFWBz</t>
-  </si>
-  <si>
-    <t>YYBNWf</t>
-  </si>
-  <si>
-    <t>YYNWFw</t>
-  </si>
-  <si>
-    <t>YYWFWb</t>
-  </si>
-  <si>
     <t>YYWNWl</t>
   </si>
   <si>
@@ -154,9 +142,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -245,15 +227,6 @@
   </si>
   <si>
     <t>YAAAA</t>
-  </si>
-  <si>
-    <t>YYFWB</t>
-  </si>
-  <si>
-    <t>YYNWF</t>
-  </si>
-  <si>
-    <t>YYWFW</t>
   </si>
   <si>
     <t>YYWNW</t>
@@ -644,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,22 +628,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -678,22 +651,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -701,22 +674,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -724,22 +697,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -747,22 +720,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -770,22 +743,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -793,22 +766,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -816,22 +789,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -839,22 +812,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -862,22 +835,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -885,22 +858,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -908,22 +881,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -931,22 +904,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -954,22 +927,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -977,22 +950,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1000,22 +973,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1023,22 +996,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
         <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1046,22 +1019,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1069,22 +1042,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1092,22 +1065,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1115,22 +1088,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1138,22 +1111,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1161,22 +1134,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1184,22 +1157,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1207,19 +1180,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
         <v>50</v>
@@ -1230,22 +1203,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1253,22 +1226,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
         <v>43</v>
-      </c>
-      <c r="G27" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1276,22 +1249,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G28" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1299,22 +1272,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" t="s">
         <v>43</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1322,22 +1295,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1345,19 +1318,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G31" t="s">
         <v>48</v>
@@ -1368,22 +1341,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1391,22 +1364,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1414,114 +1387,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
         <v>43</v>
-      </c>
-      <c r="G34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" t="s">
-        <v>44</v>
-      </c>
-      <c r="G38" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1412,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1542,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1553,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1564,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1575,7 +1456,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1586,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1597,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1608,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1619,7 +1500,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1630,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1641,7 +1522,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1652,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1663,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1674,7 +1555,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1685,7 +1566,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1696,7 +1577,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1707,7 +1588,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1718,7 +1599,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1729,7 +1610,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1740,7 +1621,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1751,7 +1632,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1762,7 +1643,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1773,7 +1654,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1784,7 +1665,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1795,7 +1676,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1806,7 +1687,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1817,7 +1698,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1828,7 +1709,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1839,7 +1720,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1850,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1861,7 +1742,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1872,7 +1753,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1883,7 +1764,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1894,7 +1775,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1905,53 +1786,9 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38">
         <v>1</v>
       </c>
     </row>
@@ -1962,7 +1799,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1973,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1984,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1995,7 +1832,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2006,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2017,7 +1854,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2028,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2039,7 +1876,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2050,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2061,7 +1898,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2072,7 +1909,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2083,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2094,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2105,7 +1942,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2116,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2127,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2138,7 +1975,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2149,7 +1986,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2160,7 +1997,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2171,7 +2008,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2182,7 +2019,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2193,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2204,7 +2041,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2215,7 +2052,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2226,7 +2063,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2237,7 +2074,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2248,7 +2085,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2259,7 +2096,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2270,7 +2107,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2281,7 +2118,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2292,7 +2129,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2303,7 +2140,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2314,7 +2151,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2325,7 +2162,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2336,53 +2173,9 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38">
         <v>-1</v>
       </c>
     </row>
@@ -2393,7 +2186,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2401,519 +2194,519 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
         <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F26" t="s">
         <v>41</v>
@@ -2921,122 +2714,62 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rotation mask - this allows the user to mask which rotations are included which means the user can run all the rotations and then mask out the unprofitable ones which is good when using the full rot. Add rot mask to pinp. No profit change
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -82,6 +82,18 @@
     <t>YAAAAa</t>
   </si>
   <si>
+    <t>YYFWBz</t>
+  </si>
+  <si>
+    <t>YYBNWf</t>
+  </si>
+  <si>
+    <t>YYNWFw</t>
+  </si>
+  <si>
+    <t>YYWFWb</t>
+  </si>
+  <si>
     <t>YYWNWl</t>
   </si>
   <si>
@@ -142,6 +154,9 @@
     <t>W</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>L</t>
   </si>
   <si>
@@ -172,6 +187,9 @@
     <t>w</t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>l</t>
   </si>
   <si>
@@ -227,6 +245,15 @@
   </si>
   <si>
     <t>YAAAA</t>
+  </si>
+  <si>
+    <t>YYFWB</t>
+  </si>
+  <si>
+    <t>YYNWF</t>
+  </si>
+  <si>
+    <t>YYWFW</t>
   </si>
   <si>
     <t>YYWNW</t>
@@ -617,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -628,22 +655,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -651,22 +678,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -674,22 +701,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -697,22 +724,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -720,22 +747,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -743,22 +770,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -766,22 +793,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -789,22 +816,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -812,22 +839,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -835,22 +862,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -858,22 +885,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -881,22 +908,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -904,22 +931,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -927,22 +954,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -950,22 +977,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -973,22 +1000,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -996,22 +1023,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1019,22 +1046,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1042,22 +1069,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1065,22 +1092,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1088,22 +1115,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1111,22 +1138,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1134,22 +1161,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1157,22 +1184,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1180,19 +1207,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
         <v>50</v>
@@ -1203,22 +1230,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1226,22 +1253,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1249,22 +1276,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1272,22 +1299,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1295,22 +1322,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1318,19 +1345,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G31" t="s">
         <v>48</v>
@@ -1341,22 +1368,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1364,22 +1391,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1387,22 +1414,114 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" t="s">
-        <v>43</v>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1423,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1434,7 +1553,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1445,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1456,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1467,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1478,7 +1597,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1489,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1500,7 +1619,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1511,7 +1630,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1522,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1533,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1544,7 +1663,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1555,7 +1674,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1566,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1577,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1588,7 +1707,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1599,7 +1718,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1610,7 +1729,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1621,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1632,7 +1751,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1643,7 +1762,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1654,7 +1773,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1665,7 +1784,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1676,7 +1795,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1687,7 +1806,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1698,7 +1817,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1709,7 +1828,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1720,7 +1839,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1731,7 +1850,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1742,7 +1861,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1753,7 +1872,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1764,7 +1883,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1775,7 +1894,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1786,9 +1905,53 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
     </row>
@@ -1799,7 +1962,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1810,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1821,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1832,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -1843,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -1854,7 +2017,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -1865,7 +2028,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -1876,7 +2039,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -1887,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1898,7 +2061,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -1909,7 +2072,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -1920,7 +2083,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1931,7 +2094,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1942,7 +2105,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1953,7 +2116,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1964,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1975,7 +2138,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1986,7 +2149,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1997,7 +2160,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2008,7 +2171,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2019,7 +2182,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2030,7 +2193,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2041,7 +2204,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2052,7 +2215,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2063,7 +2226,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2074,7 +2237,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2085,7 +2248,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2096,7 +2259,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2107,7 +2270,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2118,7 +2281,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2129,7 +2292,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2140,7 +2303,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2151,7 +2314,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2162,7 +2325,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2173,9 +2336,53 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38">
         <v>-1</v>
       </c>
     </row>
@@ -2186,7 +2393,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2194,519 +2401,519 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
         <v>41</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
         <v>41</v>
@@ -2714,62 +2921,122 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update rot.xl and var sum due to a2 landuse. Profit increased a bit which is because a2 has no costs. Later it will get masked out and the profit will reduce again.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,11 +17,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="111">
   <si>
     <t>AAAAAa</t>
   </si>
   <si>
+    <t>GGGGAa2</t>
+  </si>
+  <si>
+    <t>GGGANa2</t>
+  </si>
+  <si>
+    <t>GGGAEa2</t>
+  </si>
+  <si>
+    <t>GGGAOFa2</t>
+  </si>
+  <si>
+    <t>GGGC1Na2</t>
+  </si>
+  <si>
+    <t>GGGC1Ea2</t>
+  </si>
+  <si>
+    <t>GGGC1Pa2</t>
+  </si>
+  <si>
+    <t>GGGC1OFa2</t>
+  </si>
+  <si>
     <t>SPSPSPSPSPsp</t>
   </si>
   <si>
@@ -136,6 +160,9 @@
     <t>A</t>
   </si>
   <si>
+    <t>G</t>
+  </si>
+  <si>
     <t>SP</t>
   </si>
   <si>
@@ -160,12 +187,24 @@
     <t>L</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>OF</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
+    <t>a2</t>
+  </si>
+  <si>
     <t>sp</t>
   </si>
   <si>
@@ -194,6 +233,30 @@
   </si>
   <si>
     <t>AAAAA</t>
+  </si>
+  <si>
+    <t>GGGGA</t>
+  </si>
+  <si>
+    <t>GGGAN</t>
+  </si>
+  <si>
+    <t>GGGAE</t>
+  </si>
+  <si>
+    <t>GGGAOF</t>
+  </si>
+  <si>
+    <t>GGGC1N</t>
+  </si>
+  <si>
+    <t>GGGC1E</t>
+  </si>
+  <si>
+    <t>GGGC1P</t>
+  </si>
+  <si>
+    <t>GGGC1OF</t>
   </si>
   <si>
     <t>SPSPSPSPSP</t>
@@ -644,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,22 +718,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -678,22 +741,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -701,22 +764,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -724,22 +787,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -747,22 +810,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -770,22 +833,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -793,22 +856,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -816,22 +879,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -839,22 +902,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -862,22 +925,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -885,22 +948,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -908,22 +971,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -931,22 +994,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -954,22 +1017,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -977,22 +1040,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1000,22 +1063,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1023,22 +1086,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1046,22 +1109,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1069,22 +1132,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1092,22 +1155,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1115,22 +1178,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1138,22 +1201,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1161,22 +1224,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1184,22 +1247,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1207,22 +1270,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1230,22 +1293,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1253,22 +1316,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1276,22 +1339,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
         <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1299,22 +1362,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
         <v>46</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1322,22 +1385,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1345,22 +1408,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1368,22 +1431,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1391,22 +1454,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1414,22 +1477,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1437,22 +1500,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G35" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1460,22 +1523,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1483,22 +1546,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1506,22 +1569,206 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F38" t="s">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G38" t="s">
-        <v>48</v>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1778,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1542,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1553,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1564,7 +1811,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1575,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1586,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1597,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1608,7 +1855,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1619,7 +1866,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1630,7 +1877,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1641,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1652,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1663,7 +1910,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1674,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1685,7 +1932,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1696,7 +1943,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1707,7 +1954,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1718,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1729,7 +1976,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1740,7 +1987,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1751,7 +1998,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1762,7 +2009,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1773,7 +2020,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1784,7 +2031,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1795,7 +2042,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1806,7 +2053,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1817,7 +2064,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1828,7 +2075,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1839,7 +2086,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1850,7 +2097,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1861,7 +2108,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1872,7 +2119,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1883,7 +2130,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1894,7 +2141,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1905,7 +2152,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1916,7 +2163,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1927,7 +2174,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1938,7 +2185,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1949,9 +2196,97 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46">
         <v>1</v>
       </c>
     </row>
@@ -1962,7 +2297,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1973,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -1981,10 +2316,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -1992,10 +2327,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2003,10 +2338,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2014,10 +2349,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2025,10 +2360,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2036,10 +2371,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2047,10 +2382,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2058,10 +2393,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2069,10 +2404,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2080,10 +2415,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2091,10 +2426,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2102,10 +2437,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2113,10 +2448,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2124,10 +2459,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2138,7 +2473,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2149,7 +2484,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2157,10 +2492,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2168,10 +2503,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2179,10 +2514,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2190,10 +2525,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2201,10 +2536,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2212,7 +2547,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
@@ -2223,10 +2558,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -2234,10 +2569,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -2245,10 +2580,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2256,10 +2591,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -2267,10 +2602,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -2278,10 +2613,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2289,10 +2624,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2300,10 +2635,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2311,10 +2646,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2322,10 +2657,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -2333,10 +2668,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -2344,10 +2679,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -2355,10 +2690,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -2366,10 +2701,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2377,12 +2712,430 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38">
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76">
         <v>-1</v>
       </c>
     </row>
@@ -2393,7 +3146,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2401,559 +3154,559 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
         <v>46</v>
@@ -2961,82 +3714,242 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweak rotation so that a2 (pnc) is included in history constraint but it doesnt provide a history which forces the model to change landuse. Also tweak so that rotation phases require more general histories, this is how the google doc explains it so not sure why it is not correct in the code - this hasnt previously been an issue because rotations have only provided one hist and required one hist but when pnc was added now phases can provide multiple histories and therefore have to req multiple histories..
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="111">
   <si>
     <t>AAAAAa</t>
   </si>
@@ -1778,7 +1778,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
@@ -1808,10 +1808,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1819,10 +1819,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1830,10 +1830,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1863,10 +1863,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1874,10 +1874,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1885,10 +1885,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1907,10 +1907,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1918,10 +1918,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1951,10 +1951,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1962,10 +1962,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1973,10 +1973,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2028,10 +2028,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2083,10 +2083,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2094,10 +2094,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2105,10 +2105,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2127,10 +2127,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2149,10 +2149,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2171,10 +2171,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2182,10 +2182,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2193,10 +2193,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2204,10 +2204,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2215,10 +2215,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2237,10 +2237,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2248,10 +2248,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2259,10 +2259,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2270,10 +2270,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2281,12 +2281,452 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" t="s">
+        <v>73</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" t="s">
+        <v>72</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B85" t="s">
         <v>91</v>
       </c>
-      <c r="C46">
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>45</v>
+      </c>
+      <c r="B86" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweak rotation generation so that it works correctly. Had to number some landuse sets to stop provide/req in the incorect history yr. Also add germination reduction for pasture following S (this required adding a pnc phase). Added a test to pick up and remove rotations with a history that isnt provided by any other rotation (this is requireed for phases like YNOS1z that cant be provided due to needing an annual in yr5 but only canola can follow annual but yr3 is cannola so yr4 cant be canola) Redo sim inputs accordingly to match the new rotations and sets. Create rotation mask.
</commit_message>
<xml_diff>
--- a/Rotation.xlsx
+++ b/Rotation.xlsx
@@ -17,21 +17,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="111">
-  <si>
-    <t>AAAAAa</t>
-  </si>
-  <si>
-    <t>GGGGAa2</t>
-  </si>
-  <si>
-    <t>GGGANa2</t>
-  </si>
-  <si>
-    <t>GGGAEa2</t>
-  </si>
-  <si>
-    <t>GGGAOFa2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="118">
+  <si>
+    <t>AAAA2A1a</t>
+  </si>
+  <si>
+    <t>GGGGAg1a2</t>
+  </si>
+  <si>
+    <t>GGGGSg1a2</t>
+  </si>
+  <si>
+    <t>GGGAg2Na2</t>
+  </si>
+  <si>
+    <t>GGGAg2Ea2</t>
+  </si>
+  <si>
+    <t>GGGAg2OFa2</t>
   </si>
   <si>
     <t>GGGC1Na2</t>
@@ -49,19 +52,19 @@
     <t>SPSPSPSPSPsp</t>
   </si>
   <si>
-    <t>YABABa</t>
-  </si>
-  <si>
-    <t>AYABAb</t>
-  </si>
-  <si>
-    <t>AYABAbd</t>
-  </si>
-  <si>
-    <t>YAOAOFa</t>
-  </si>
-  <si>
-    <t>AYAOAof</t>
+    <t>YABA2Ba</t>
+  </si>
+  <si>
+    <t>AYABA1b</t>
+  </si>
+  <si>
+    <t>AYABA1bd</t>
+  </si>
+  <si>
+    <t>YAOA2OFa</t>
+  </si>
+  <si>
+    <t>AYAOA1of</t>
   </si>
   <si>
     <t>YYNBNb</t>
@@ -82,10 +85,10 @@
     <t>YYBNWb</t>
   </si>
   <si>
-    <t>AAAAAz</t>
-  </si>
-  <si>
-    <t>AAAANw</t>
+    <t>AAAA2A1z</t>
+  </si>
+  <si>
+    <t>AAAA2Nw</t>
   </si>
   <si>
     <t>AAANWb</t>
@@ -94,16 +97,16 @@
     <t>AANWBa</t>
   </si>
   <si>
-    <t>AYWBAa</t>
-  </si>
-  <si>
-    <t>YYBAAa</t>
-  </si>
-  <si>
-    <t>YYAAAa</t>
-  </si>
-  <si>
-    <t>YAAAAa</t>
+    <t>AYWBA1a</t>
+  </si>
+  <si>
+    <t>YYBA2A1a</t>
+  </si>
+  <si>
+    <t>YYAA2A1a</t>
+  </si>
+  <si>
+    <t>YAAA2A1a</t>
   </si>
   <si>
     <t>YYFWBz</t>
@@ -130,28 +133,28 @@
     <t>YYNWLw</t>
   </si>
   <si>
-    <t>AYAAAw</t>
-  </si>
-  <si>
-    <t>AAWAAa</t>
-  </si>
-  <si>
-    <t>AAAWAa</t>
-  </si>
-  <si>
-    <t>YAAAWa</t>
-  </si>
-  <si>
-    <t>YAAANw</t>
-  </si>
-  <si>
-    <t>AYAAAz</t>
-  </si>
-  <si>
-    <t>AYWAAa</t>
-  </si>
-  <si>
-    <t>AANWAa</t>
+    <t>AYAA2A1w</t>
+  </si>
+  <si>
+    <t>AAWA2A1a</t>
+  </si>
+  <si>
+    <t>AAAWA1a</t>
+  </si>
+  <si>
+    <t>YAAA2Wa</t>
+  </si>
+  <si>
+    <t>YAAA2Nw</t>
+  </si>
+  <si>
+    <t>YYAA2A1z</t>
+  </si>
+  <si>
+    <t>AYWA2A1a</t>
+  </si>
+  <si>
+    <t>AANWA1a</t>
   </si>
   <si>
     <t>AAANWa</t>
@@ -187,9 +190,24 @@
     <t>L</t>
   </si>
   <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Ag2</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Ag1</t>
+  </si>
+  <si>
+    <t>Sg1</t>
+  </si>
+  <si>
     <t>E</t>
   </si>
   <si>
@@ -232,19 +250,22 @@
     <t>l</t>
   </si>
   <si>
-    <t>AAAAA</t>
-  </si>
-  <si>
-    <t>GGGGA</t>
-  </si>
-  <si>
-    <t>GGGAN</t>
-  </si>
-  <si>
-    <t>GGGAE</t>
-  </si>
-  <si>
-    <t>GGGAOF</t>
+    <t>AAAA2A1</t>
+  </si>
+  <si>
+    <t>GGGGAg1</t>
+  </si>
+  <si>
+    <t>GGGGSg1</t>
+  </si>
+  <si>
+    <t>GGGAg2N</t>
+  </si>
+  <si>
+    <t>GGGAg2E</t>
+  </si>
+  <si>
+    <t>GGGAg2OF</t>
   </si>
   <si>
     <t>GGGC1N</t>
@@ -262,16 +283,16 @@
     <t>SPSPSPSPSP</t>
   </si>
   <si>
-    <t>YABAB</t>
-  </si>
-  <si>
-    <t>AYABA</t>
-  </si>
-  <si>
-    <t>YAOAOF</t>
-  </si>
-  <si>
-    <t>AYAOA</t>
+    <t>YABA2B</t>
+  </si>
+  <si>
+    <t>AYABA1</t>
+  </si>
+  <si>
+    <t>YAOA2OF</t>
+  </si>
+  <si>
+    <t>AYAOA1</t>
   </si>
   <si>
     <t>YYNBN</t>
@@ -289,7 +310,7 @@
     <t>YYBNW</t>
   </si>
   <si>
-    <t>AAAAN</t>
+    <t>AAAA2N</t>
   </si>
   <si>
     <t>AAANW</t>
@@ -298,16 +319,16 @@
     <t>AANWB</t>
   </si>
   <si>
-    <t>AYWBA</t>
-  </si>
-  <si>
-    <t>YYBAA</t>
-  </si>
-  <si>
-    <t>YYAAA</t>
-  </si>
-  <si>
-    <t>YAAAA</t>
+    <t>AYWBA1</t>
+  </si>
+  <si>
+    <t>YYBA2A1</t>
+  </si>
+  <si>
+    <t>YYAA2A1</t>
+  </si>
+  <si>
+    <t>YAAA2A1</t>
   </si>
   <si>
     <t>YYFWB</t>
@@ -331,25 +352,25 @@
     <t>YYNWL</t>
   </si>
   <si>
-    <t>AYAAA</t>
-  </si>
-  <si>
-    <t>AAWAA</t>
-  </si>
-  <si>
-    <t>AAAWA</t>
-  </si>
-  <si>
-    <t>YAAAW</t>
-  </si>
-  <si>
-    <t>YAAAN</t>
-  </si>
-  <si>
-    <t>AYWAA</t>
-  </si>
-  <si>
-    <t>AANWA</t>
+    <t>AYAA2A1</t>
+  </si>
+  <si>
+    <t>AAWA2A1</t>
+  </si>
+  <si>
+    <t>AAAWA1</t>
+  </si>
+  <si>
+    <t>YAAA2W</t>
+  </si>
+  <si>
+    <t>YAAA2N</t>
+  </si>
+  <si>
+    <t>AYWA2A1</t>
+  </si>
+  <si>
+    <t>AANWA1</t>
   </si>
 </sst>
 </file>
@@ -707,7 +728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,22 +739,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -741,22 +762,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -764,22 +785,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -787,22 +808,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -810,22 +831,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -833,22 +854,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -856,22 +877,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -879,22 +900,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -902,22 +923,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -934,13 +955,13 @@
         <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -951,19 +972,19 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -971,22 +992,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -994,22 +1015,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1017,22 +1038,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1040,22 +1061,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1063,22 +1084,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1086,22 +1107,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1109,22 +1130,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1132,22 +1153,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
         <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1155,22 +1176,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1178,22 +1199,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
         <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1201,22 +1222,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1224,22 +1245,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1247,22 +1268,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
         <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1270,22 +1291,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1293,22 +1314,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1316,22 +1337,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1339,22 +1360,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1362,22 +1383,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G29" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1385,19 +1406,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G30" t="s">
         <v>66</v>
@@ -1408,22 +1429,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1431,13 +1452,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
         <v>53</v>
@@ -1446,7 +1467,7 @@
         <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1454,10 +1475,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
         <v>53</v>
@@ -1466,10 +1487,10 @@
         <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1477,22 +1498,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1500,22 +1521,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1523,22 +1544,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1546,22 +1567,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1569,22 +1590,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G38" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1592,22 +1613,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F39" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G39" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1615,22 +1636,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G40" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1638,22 +1659,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1661,22 +1682,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F42" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1684,22 +1705,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E43" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F43" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G43" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1707,22 +1728,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E44" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G44" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1730,22 +1751,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G45" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1753,22 +1774,45 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" t="s">
         <v>53</v>
       </c>
-      <c r="G46" t="s">
-        <v>60</v>
+      <c r="F47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1778,7 +1822,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1789,7 +1833,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1800,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1811,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1822,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1833,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1844,7 +1888,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1852,10 +1896,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1866,7 +1910,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1877,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1888,7 +1932,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1899,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1907,10 +1951,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1921,7 +1965,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1932,7 +1976,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1940,7 +1984,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>81</v>
@@ -1954,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1962,10 +2006,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1976,7 +2020,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1984,10 +2028,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1998,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2006,10 +2050,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2017,10 +2061,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2031,7 +2075,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2039,10 +2083,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2053,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2061,10 +2105,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2075,7 +2119,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2083,10 +2127,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2097,7 +2141,7 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2105,10 +2149,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2119,7 +2163,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2127,10 +2171,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2141,7 +2185,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2149,10 +2193,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2163,7 +2207,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2171,10 +2215,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2185,7 +2229,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2193,10 +2237,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2207,7 +2251,7 @@
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2215,10 +2259,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2229,7 +2273,7 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2237,10 +2281,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2251,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2259,10 +2303,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2273,7 +2317,7 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2281,10 +2325,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2295,7 +2339,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2303,10 +2347,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2317,7 +2361,7 @@
         <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2325,10 +2369,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2339,7 +2383,7 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2347,10 +2391,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2361,7 +2405,7 @@
         <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2369,10 +2413,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2383,7 +2427,7 @@
         <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2391,10 +2435,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2405,7 +2449,7 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2413,10 +2457,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2427,7 +2471,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2435,10 +2479,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2449,7 +2493,7 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2457,10 +2501,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2471,7 +2515,7 @@
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2479,10 +2523,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2493,7 +2537,7 @@
         <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2501,10 +2545,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2515,7 +2559,7 @@
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2523,10 +2567,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2537,7 +2581,7 @@
         <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2545,10 +2589,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2559,7 +2603,7 @@
         <v>38</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2567,10 +2611,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2581,7 +2625,7 @@
         <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2589,10 +2633,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2603,7 +2647,7 @@
         <v>40</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -2611,10 +2655,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -2625,7 +2669,7 @@
         <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2633,10 +2677,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2647,7 +2691,7 @@
         <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -2655,10 +2699,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2669,7 +2713,7 @@
         <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -2677,10 +2721,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2691,7 +2735,7 @@
         <v>44</v>
       </c>
       <c r="B83" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2699,10 +2743,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2713,7 +2757,7 @@
         <v>45</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -2721,12 +2765,23 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87">
         <v>1</v>
       </c>
     </row>
@@ -2748,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -2759,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -2767,10 +2822,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2778,10 +2833,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2789,10 +2844,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2800,10 +2855,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2811,10 +2866,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2822,10 +2877,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2833,10 +2888,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2844,10 +2899,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2855,10 +2910,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2866,10 +2921,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2877,10 +2932,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2888,10 +2943,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2899,10 +2954,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2910,10 +2965,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2921,10 +2976,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2932,10 +2987,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2943,10 +2998,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2954,10 +3009,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2965,10 +3020,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -2976,10 +3031,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -2987,10 +3042,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -2998,10 +3053,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -3009,10 +3064,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -3020,10 +3075,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -3031,10 +3086,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -3042,10 +3097,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -3053,10 +3108,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -3064,10 +3119,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -3075,10 +3130,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -3086,10 +3141,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -3097,10 +3152,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -3108,10 +3163,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -3119,10 +3174,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -3130,10 +3185,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -3141,10 +3196,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -3152,10 +3207,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -3163,10 +3218,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -3174,10 +3229,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -3185,10 +3240,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -3196,10 +3251,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C42">
         <v>-1</v>
@@ -3207,10 +3262,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C43">
         <v>-1</v>
@@ -3218,10 +3273,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C44">
         <v>-1</v>
@@ -3229,10 +3284,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C45">
         <v>-1</v>
@@ -3240,10 +3295,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C46">
         <v>-1</v>
@@ -3251,10 +3306,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C47">
         <v>-1</v>
@@ -3262,10 +3317,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C48">
         <v>-1</v>
@@ -3273,10 +3328,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C49">
         <v>-1</v>
@@ -3284,10 +3339,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -3295,10 +3350,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C51">
         <v>-1</v>
@@ -3306,10 +3361,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C52">
         <v>-1</v>
@@ -3317,10 +3372,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C53">
         <v>-1</v>
@@ -3328,10 +3383,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>-1</v>
@@ -3339,10 +3394,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C55">
         <v>-1</v>
@@ -3350,10 +3405,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -3361,10 +3416,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C57">
         <v>-1</v>
@@ -3372,10 +3427,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3383,10 +3438,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -3394,10 +3449,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C60">
         <v>-1</v>
@@ -3405,10 +3460,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C61">
         <v>-1</v>
@@ -3416,10 +3471,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C62">
         <v>-1</v>
@@ -3427,10 +3482,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C63">
         <v>-1</v>
@@ -3438,10 +3493,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -3449,10 +3504,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C65">
         <v>-1</v>
@@ -3460,10 +3515,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C66">
         <v>-1</v>
@@ -3471,10 +3526,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C67">
         <v>-1</v>
@@ -3482,10 +3537,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C68">
         <v>-1</v>
@@ -3493,10 +3548,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C69">
         <v>-1</v>
@@ -3504,10 +3559,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -3515,10 +3570,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C71">
         <v>-1</v>
@@ -3526,10 +3581,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C72">
         <v>-1</v>
@@ -3537,10 +3592,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C73">
         <v>-1</v>
@@ -3548,10 +3603,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C74">
         <v>-1</v>
@@ -3559,10 +3614,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C75">
         <v>-1</v>
@@ -3570,10 +3625,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C76">
         <v>-1</v>
@@ -3586,7 +3641,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3594,407 +3649,407 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
@@ -4009,64 +4064,64 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
         <v>53</v>
@@ -4074,239 +4129,239 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" t="s">
         <v>53</v>
-      </c>
-      <c r="F34" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
         <v>55</v>
@@ -4314,39 +4369,39 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
         <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -4354,42 +4409,62 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
         <v>55</v>
       </c>
       <c r="F39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" t="s">
         <v>53</v>
       </c>
-      <c r="E40" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" t="s">
-        <v>53</v>
+      <c r="F41" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>